<commit_message>
222 in both .py and .xlsx
</commit_message>
<xml_diff>
--- a/binary.xlsx
+++ b/binary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\MergeTest1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B876C463-F37A-4D6B-9DAB-AE4012DF2DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44F3FA5-0EFE-4D8A-A7E6-5715B89F23EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -340,14 +340,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>111</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
333 in both .py and .xlsx
</commit_message>
<xml_diff>
--- a/binary.xlsx
+++ b/binary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\MergeTest1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B876C463-F37A-4D6B-9DAB-AE4012DF2DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE842E50-D71E-45BA-A6D7-757522E0D4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -347,7 +347,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>111</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>